<commit_message>
remove highlights previous changes
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_3/1_3_yearly_rep.xlsx
+++ b/dictionaries/outcome_ath/1_3/1_3_yearly_rep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\ds-dictionaries\dictionaries\outcome_ath\1_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293CF76B-D078-4423-89C7-EB8E5E43124B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D2C624-D031-41AB-B951-2D8371B6A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -796,12 +796,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1122,14 +1123,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView showFormulas="1" showGridLines="0" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
-    </sheetView>
+    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="29.1328125" customWidth="1"/>
-    <col min="2" max="3" width="15.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" customWidth="1"/>
     <col min="4" max="4" width="97.86328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1137,7 +1137,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1151,7 +1151,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -1165,7 +1165,7 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
@@ -1176,7 +1176,7 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
@@ -1190,7 +1190,7 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
@@ -1204,7 +1204,7 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
@@ -1218,7 +1218,7 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
@@ -1232,7 +1232,7 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
@@ -1246,7 +1246,7 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C9" t="s">
@@ -1260,7 +1260,7 @@
       <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
@@ -1274,7 +1274,7 @@
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
@@ -1288,7 +1288,7 @@
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" t="s">
@@ -1302,7 +1302,7 @@
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
@@ -1316,7 +1316,7 @@
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C14" t="s">
@@ -1330,7 +1330,7 @@
       <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
@@ -1344,7 +1344,7 @@
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
@@ -1355,7 +1355,7 @@
       <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
@@ -1369,7 +1369,7 @@
       <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
@@ -1383,7 +1383,7 @@
       <c r="A19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
@@ -1397,7 +1397,7 @@
       <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C20" t="s">
@@ -1411,7 +1411,7 @@
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C21" t="s">
@@ -1425,7 +1425,7 @@
       <c r="A22" t="s">
         <v>48</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C22" t="s">
@@ -1439,7 +1439,7 @@
       <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C23" t="s">
@@ -1453,7 +1453,7 @@
       <c r="A24" t="s">
         <v>52</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C24" t="s">
@@ -1467,7 +1467,7 @@
       <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C25" t="s">
@@ -1481,7 +1481,7 @@
       <c r="A26" t="s">
         <v>56</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
@@ -1495,7 +1495,7 @@
       <c r="A27" t="s">
         <v>57</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C27" t="s">
@@ -1509,7 +1509,7 @@
       <c r="A28" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D28" t="s">
@@ -1520,7 +1520,7 @@
       <c r="A29" t="s">
         <v>61</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C29" t="s">
@@ -1534,7 +1534,7 @@
       <c r="A30" t="s">
         <v>63</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C30" t="s">
@@ -1548,7 +1548,7 @@
       <c r="A31" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D31" t="s">
@@ -1559,7 +1559,7 @@
       <c r="A32" t="s">
         <v>67</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C32" t="s">
@@ -1573,7 +1573,7 @@
       <c r="A33" t="s">
         <v>69</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C33" t="s">
@@ -1587,7 +1587,7 @@
       <c r="A34" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D34" t="s">
@@ -1598,7 +1598,7 @@
       <c r="A35" t="s">
         <v>73</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C35" t="s">
@@ -1612,7 +1612,7 @@
       <c r="A36" t="s">
         <v>75</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C36" t="s">
@@ -1626,7 +1626,7 @@
       <c r="A37" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D37" t="s">
@@ -1637,7 +1637,7 @@
       <c r="A38" t="s">
         <v>79</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C38" t="s">
@@ -1651,7 +1651,7 @@
       <c r="A39" t="s">
         <v>81</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C39" t="s">
@@ -1665,7 +1665,7 @@
       <c r="A40" t="s">
         <v>83</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C40" t="s">
@@ -1679,7 +1679,7 @@
       <c r="A41" t="s">
         <v>85</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C41" t="s">
@@ -1693,7 +1693,7 @@
       <c r="A42" t="s">
         <v>87</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C42" t="s">
@@ -1707,7 +1707,7 @@
       <c r="A43" t="s">
         <v>89</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C43" t="s">
@@ -1721,7 +1721,7 @@
       <c r="A44" t="s">
         <v>91</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C44" t="s">
@@ -1735,7 +1735,7 @@
       <c r="A45" t="s">
         <v>93</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C45" t="s">
@@ -1749,7 +1749,7 @@
       <c r="A46" t="s">
         <v>95</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C46" t="s">
@@ -1763,7 +1763,7 @@
       <c r="A47" t="s">
         <v>97</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
@@ -1777,7 +1777,7 @@
       <c r="A48" t="s">
         <v>99</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C48" t="s">
@@ -1791,7 +1791,7 @@
       <c r="A49" t="s">
         <v>101</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C49" t="s">
@@ -1805,7 +1805,7 @@
       <c r="A50" t="s">
         <v>103</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C50" t="s">
@@ -1819,7 +1819,7 @@
       <c r="A51" t="s">
         <v>105</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C51" t="s">
@@ -1833,7 +1833,7 @@
       <c r="A52" t="s">
         <v>107</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C52" t="s">
@@ -1847,7 +1847,7 @@
       <c r="A53" t="s">
         <v>109</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C53" t="s">
@@ -1861,7 +1861,7 @@
       <c r="A54" t="s">
         <v>111</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C54" t="s">
@@ -1875,7 +1875,7 @@
       <c r="A55" t="s">
         <v>113</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C55" t="s">
@@ -1889,7 +1889,7 @@
       <c r="A56" t="s">
         <v>115</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C56" t="s">
@@ -1903,7 +1903,7 @@
       <c r="A57" t="s">
         <v>118</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C57" t="s">
@@ -1917,7 +1917,7 @@
       <c r="A58" t="s">
         <v>120</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D58" t="s">
@@ -1928,7 +1928,7 @@
       <c r="A59" t="s">
         <v>122</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D59" t="s">
@@ -1939,7 +1939,7 @@
       <c r="A60" t="s">
         <v>124</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D60" t="s">
@@ -1950,7 +1950,7 @@
       <c r="A61" t="s">
         <v>126</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D61" t="s">
@@ -1958,10 +1958,10 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D62" t="s">
@@ -1972,7 +1972,7 @@
       <c r="A63" t="s">
         <v>130</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D63" t="s">
@@ -1983,7 +1983,7 @@
       <c r="A64" t="s">
         <v>132</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D64" t="s">
@@ -1994,7 +1994,7 @@
       <c r="A65" t="s">
         <v>134</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D65" t="s">
@@ -2005,7 +2005,7 @@
       <c r="A66" t="s">
         <v>136</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D66" t="s">
@@ -2016,7 +2016,7 @@
       <c r="A67" t="s">
         <v>138</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D67" t="s">
@@ -2027,7 +2027,7 @@
       <c r="A68" t="s">
         <v>140</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D68" t="s">
@@ -2038,7 +2038,7 @@
       <c r="A69" t="s">
         <v>142</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D69" t="s">
@@ -2049,7 +2049,7 @@
       <c r="A70" t="s">
         <v>144</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D70" t="s">
@@ -2060,7 +2060,7 @@
       <c r="A71" t="s">
         <v>146</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D71" t="s">
@@ -2071,7 +2071,7 @@
       <c r="A72" t="s">
         <v>148</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D72" t="s">
@@ -2082,7 +2082,7 @@
       <c r="A73" t="s">
         <v>150</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D73" t="s">
@@ -2093,7 +2093,7 @@
       <c r="A74" t="s">
         <v>152</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C74" t="s">
@@ -2107,7 +2107,7 @@
       <c r="A75" t="s">
         <v>155</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C75" t="s">
@@ -2121,7 +2121,7 @@
       <c r="A76" t="s">
         <v>157</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C76" t="s">
@@ -2135,7 +2135,7 @@
       <c r="A77" t="s">
         <v>159</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C77" t="s">
@@ -2149,7 +2149,7 @@
       <c r="A78" t="s">
         <v>161</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D78" t="s">
@@ -2160,7 +2160,7 @@
       <c r="A79" t="s">
         <v>163</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C79" t="s">
@@ -2174,7 +2174,7 @@
       <c r="A80" t="s">
         <v>166</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C80" t="s">
@@ -2188,7 +2188,7 @@
       <c r="A81" t="s">
         <v>169</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D81" t="s">
@@ -2199,7 +2199,7 @@
       <c r="A82" t="s">
         <v>171</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D82" t="s">
@@ -2210,7 +2210,7 @@
       <c r="A83" t="s">
         <v>173</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D83" t="s">
@@ -2221,7 +2221,7 @@
       <c r="A84" t="s">
         <v>175</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D84" t="s">
@@ -2232,7 +2232,7 @@
       <c r="A85" t="s">
         <v>177</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D85" t="s">
@@ -2243,7 +2243,7 @@
       <c r="A86" t="s">
         <v>179</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D86" t="s">
@@ -2251,10 +2251,10 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D87" t="s">
@@ -2282,8 +2282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D336"/>
   <sheetViews>
-    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView showFormulas="1" showGridLines="0" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2981,7 +2981,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+      <c r="A50" s="4" t="s">
         <v>207</v>
       </c>
       <c r="B50">
@@ -2995,7 +2995,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="A51" s="4" t="s">
         <v>207</v>
       </c>
       <c r="B51">

</xml_diff>

<commit_message>
new cardio vars to outcome dict
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_3/1_3_yearly_rep.xlsx
+++ b/dictionaries/outcome_ath/1_3/1_3_yearly_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\ds-dictionaries\dictionaries\outcome_ath\1_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\extender_outcomes_ath\20240227updateCardio\1_3mio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D2C624-D031-41AB-B951-2D8371B6A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609C34C1-0F9B-454A-95B0-57D647EAD360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$D$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -97,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="226">
   <si>
     <t>name</t>
   </si>
@@ -721,6 +716,60 @@
   </si>
   <si>
     <t>mets_score_partial_idefics_</t>
+  </si>
+  <si>
+    <t>bmi_idefics_perc_</t>
+  </si>
+  <si>
+    <t>Repeated measures of child's BMI z-score percentiles based on the IDEFICS study reference values</t>
+  </si>
+  <si>
+    <t>bmi_idefics_z_</t>
+  </si>
+  <si>
+    <t>Repeated measures of child's BMI z-score  based on the IDEFICS study reference values</t>
+  </si>
+  <si>
+    <t>wc_idefics_z_</t>
+  </si>
+  <si>
+    <t>Repeated measures of child's waist circumference z-score  based on the IDEFICS study reference values</t>
+  </si>
+  <si>
+    <t>hdl_idefics_z_</t>
+  </si>
+  <si>
+    <t>Repeated measures of child's HDL z-score  based on the IDEFICS study reference values</t>
+  </si>
+  <si>
+    <t>triglyceride_idefics_z_</t>
+  </si>
+  <si>
+    <t>Repeated measures of child's triglycerides z-score  based on the IDEFICS study reference values</t>
+  </si>
+  <si>
+    <t>glucose_idefics_z_</t>
+  </si>
+  <si>
+    <t>Repeated measures of child's glucose z-score  based on the IDEFICS study reference values</t>
+  </si>
+  <si>
+    <t>sbp_idefics_z_</t>
+  </si>
+  <si>
+    <t>Repeated measures of child's SBP z-score  based on the IDEFICS study reference values</t>
+  </si>
+  <si>
+    <t>dbp_idefics_z_</t>
+  </si>
+  <si>
+    <t>Repeated measures of child's DBP z-score  based on the IDEFICS study reference values</t>
+  </si>
+  <si>
+    <t>mets_nriskfactors_idefics_</t>
+  </si>
+  <si>
+    <t>risk factors based on the IDEFICS study reference values</t>
   </si>
 </sst>
 </file>
@@ -796,13 +845,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,7 +875,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1121,19 +1171,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:D96"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.1328125" customWidth="1"/>
-    <col min="2" max="2" width="15.3984375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.3984375" customWidth="1"/>
-    <col min="4" max="4" width="97.86328125" customWidth="1"/>
+    <col min="1" max="1" width="29.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="97.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1172,7 +1224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1186,7 +1238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1200,7 +1252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1214,7 +1266,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1228,7 +1280,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1242,7 +1294,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1256,7 +1308,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1270,7 +1322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1284,7 +1336,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1298,7 +1350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1312,7 +1364,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1326,7 +1378,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1340,7 +1392,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1351,7 +1403,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1365,7 +1417,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1379,7 +1431,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1393,7 +1445,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1407,7 +1459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1421,7 +1473,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1435,7 +1487,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1449,7 +1501,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1463,7 +1515,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1477,7 +1529,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1491,7 +1543,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -1505,7 +1557,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1516,7 +1568,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -1530,7 +1582,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -1544,7 +1596,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -1555,7 +1607,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -1569,7 +1621,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1583,7 +1635,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -1594,7 +1646,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -1608,7 +1660,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -1622,7 +1674,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1633,7 +1685,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -1647,7 +1699,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -1661,7 +1713,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -1675,7 +1727,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -1689,7 +1741,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -1703,7 +1755,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -1717,7 +1769,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -1731,7 +1783,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -1745,7 +1797,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -1759,7 +1811,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -1773,7 +1825,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -1787,7 +1839,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>101</v>
       </c>
@@ -1801,7 +1853,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -1815,7 +1867,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -1829,7 +1881,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>107</v>
       </c>
@@ -1843,7 +1895,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -1857,7 +1909,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -1871,7 +1923,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -1885,7 +1937,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -1899,7 +1951,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>118</v>
       </c>
@@ -1913,7 +1965,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>120</v>
       </c>
@@ -1924,7 +1976,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>122</v>
       </c>
@@ -1935,7 +1987,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -1946,7 +1998,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>126</v>
       </c>
@@ -1957,7 +2009,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>206</v>
       </c>
@@ -1968,7 +2020,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>130</v>
       </c>
@@ -1979,7 +2031,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>132</v>
       </c>
@@ -1990,7 +2042,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -2001,7 +2053,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>136</v>
       </c>
@@ -2012,7 +2064,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>138</v>
       </c>
@@ -2023,7 +2075,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>140</v>
       </c>
@@ -2034,7 +2086,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>142</v>
       </c>
@@ -2045,7 +2097,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>144</v>
       </c>
@@ -2056,7 +2108,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -2067,7 +2119,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>148</v>
       </c>
@@ -2078,7 +2130,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>150</v>
       </c>
@@ -2089,7 +2141,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>152</v>
       </c>
@@ -2103,7 +2155,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>155</v>
       </c>
@@ -2117,7 +2169,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>157</v>
       </c>
@@ -2131,7 +2183,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>159</v>
       </c>
@@ -2145,7 +2197,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>161</v>
       </c>
@@ -2156,7 +2208,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>163</v>
       </c>
@@ -2170,7 +2222,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>166</v>
       </c>
@@ -2184,7 +2236,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -2195,7 +2247,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -2206,7 +2258,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -2217,7 +2269,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>175</v>
       </c>
@@ -2228,7 +2280,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>177</v>
       </c>
@@ -2239,7 +2291,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>179</v>
       </c>
@@ -2250,7 +2302,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>207</v>
       </c>
@@ -2259,6 +2311,114 @@
       </c>
       <c r="D87" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2286,15 +2446,15 @@
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" customWidth="1"/>
-    <col min="3" max="3" width="37.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.3984375" customWidth="1"/>
+    <col min="1" max="1" width="37.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" customWidth="1"/>
+    <col min="3" max="3" width="37.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>181</v>
       </c>
@@ -2308,7 +2468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2322,7 +2482,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2336,7 +2496,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2350,7 +2510,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2364,7 +2524,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2378,7 +2538,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2392,7 +2552,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2406,7 +2566,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2420,7 +2580,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2434,7 +2594,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2448,7 +2608,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2462,7 +2622,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2476,7 +2636,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2490,7 +2650,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -2504,7 +2664,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2518,7 +2678,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2532,7 +2692,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -2546,7 +2706,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -2560,7 +2720,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -2574,7 +2734,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2588,7 +2748,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -2602,7 +2762,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2616,7 +2776,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -2630,7 +2790,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -2644,7 +2804,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -2658,7 +2818,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -2672,7 +2832,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -2686,7 +2846,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -2700,7 +2860,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2714,7 +2874,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -2728,7 +2888,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -2742,7 +2902,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2756,7 +2916,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>126</v>
       </c>
@@ -2770,7 +2930,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>126</v>
       </c>
@@ -2784,7 +2944,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>128</v>
       </c>
@@ -2798,7 +2958,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -2812,7 +2972,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>171</v>
       </c>
@@ -2826,7 +2986,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>171</v>
       </c>
@@ -2840,7 +3000,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>173</v>
       </c>
@@ -2854,7 +3014,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>173</v>
       </c>
@@ -2868,7 +3028,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>175</v>
       </c>
@@ -2882,7 +3042,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>175</v>
       </c>
@@ -2896,7 +3056,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>177</v>
       </c>
@@ -2910,7 +3070,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>177</v>
       </c>
@@ -2924,7 +3084,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>177</v>
       </c>
@@ -2938,7 +3098,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>177</v>
       </c>
@@ -2952,7 +3112,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>179</v>
       </c>
@@ -2966,7 +3126,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>179</v>
       </c>
@@ -2980,7 +3140,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>207</v>
       </c>
@@ -2994,7 +3154,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>207</v>
       </c>
@@ -3008,859 +3168,859 @@
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C120" s="1"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C121" s="1"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C123" s="1"/>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C125" s="1"/>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C126" s="1"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C127" s="1"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C128" s="1"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C129" s="1"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C130" s="1"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C132" s="1"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C133" s="1"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C134" s="1"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C135" s="1"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C136" s="1"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C137" s="1"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C138" s="1"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C139" s="1"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C140" s="1"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C141" s="1"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C142" s="1"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C143" s="1"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C144" s="1"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C145" s="1"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C150" s="1"/>
     </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C151" s="1"/>
     </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C152" s="1"/>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C153" s="1"/>
     </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C154" s="1"/>
     </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="155" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C155" s="1"/>
     </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="156" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C156" s="1"/>
     </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="157" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C157" s="1"/>
     </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="158" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C158" s="1"/>
     </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="159" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C159" s="1"/>
     </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="160" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C160" s="1"/>
     </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="161" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C161" s="1"/>
     </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="162" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C162" s="1"/>
     </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="163" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C163" s="1"/>
     </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="164" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C164" s="1"/>
     </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="165" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C165" s="1"/>
     </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="166" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C166" s="1"/>
     </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="167" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C167" s="1"/>
     </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="168" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C168" s="1"/>
     </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="169" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C169" s="1"/>
     </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="170" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C170" s="1"/>
     </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="171" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C171" s="1"/>
     </row>
-    <row r="172" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="172" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C172" s="1"/>
     </row>
-    <row r="173" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="173" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C173" s="1"/>
     </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="174" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C174" s="1"/>
     </row>
-    <row r="175" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="175" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C175" s="1"/>
     </row>
-    <row r="176" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="176" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C176" s="1"/>
     </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="177" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C177" s="1"/>
     </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="178" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C178" s="1"/>
     </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="179" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C179" s="1"/>
     </row>
-    <row r="180" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="180" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C180" s="1"/>
     </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="181" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C181" s="1"/>
     </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="182" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C182" s="1"/>
     </row>
-    <row r="183" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="183" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C183" s="1"/>
     </row>
-    <row r="184" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="184" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C184" s="1"/>
     </row>
-    <row r="185" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="185" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C185" s="1"/>
     </row>
-    <row r="186" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="186" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C186" s="1"/>
     </row>
-    <row r="187" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="187" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C187" s="1"/>
     </row>
-    <row r="188" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="188" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C188" s="1"/>
     </row>
-    <row r="189" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="189" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C189" s="1"/>
     </row>
-    <row r="190" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="190" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C190" s="1"/>
     </row>
-    <row r="191" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="191" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C191" s="1"/>
     </row>
-    <row r="192" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="192" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C192" s="1"/>
     </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="193" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C193" s="1"/>
     </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="194" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C194" s="1"/>
     </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="195" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C195" s="1"/>
     </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="196" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C196" s="1"/>
     </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="197" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C197" s="1"/>
     </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="198" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C198" s="1"/>
     </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="199" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C199" s="1"/>
     </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="200" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C200" s="1"/>
     </row>
-    <row r="201" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="201" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C201" s="1"/>
     </row>
-    <row r="202" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="202" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C202" s="1"/>
     </row>
-    <row r="203" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="203" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C203" s="1"/>
     </row>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="204" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C204" s="1"/>
     </row>
-    <row r="205" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="205" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C205" s="1"/>
     </row>
-    <row r="206" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="206" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C206" s="1"/>
     </row>
-    <row r="207" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="207" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C207" s="1"/>
     </row>
-    <row r="208" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="208" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C208" s="1"/>
     </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="209" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C209" s="1"/>
     </row>
-    <row r="210" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="210" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C210" s="1"/>
     </row>
-    <row r="211" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="211" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C211" s="1"/>
     </row>
-    <row r="212" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="212" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C212" s="1"/>
     </row>
-    <row r="213" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="213" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C213" s="1"/>
     </row>
-    <row r="214" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="214" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C214" s="1"/>
     </row>
-    <row r="215" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="215" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C215" s="1"/>
     </row>
-    <row r="216" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="216" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C216" s="1"/>
     </row>
-    <row r="217" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="217" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C217" s="1"/>
     </row>
-    <row r="218" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="218" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C218" s="1"/>
     </row>
-    <row r="219" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="219" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C219" s="1"/>
     </row>
-    <row r="220" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="220" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C220" s="1"/>
     </row>
-    <row r="221" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="221" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C221" s="1"/>
     </row>
-    <row r="222" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="222" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C222" s="1"/>
     </row>
-    <row r="223" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="223" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C223" s="1"/>
     </row>
-    <row r="224" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="224" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C224" s="1"/>
     </row>
-    <row r="225" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="225" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C225" s="1"/>
     </row>
-    <row r="226" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="226" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C226" s="1"/>
     </row>
-    <row r="227" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="227" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C227" s="1"/>
     </row>
-    <row r="228" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="228" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C228" s="1"/>
     </row>
-    <row r="229" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="229" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C229" s="1"/>
     </row>
-    <row r="230" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="230" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C230" s="1"/>
     </row>
-    <row r="231" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="231" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C231" s="1"/>
     </row>
-    <row r="232" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="232" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C232" s="1"/>
     </row>
-    <row r="233" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="233" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C233" s="1"/>
     </row>
-    <row r="234" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="234" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C234" s="1"/>
     </row>
-    <row r="235" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="235" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C235" s="1"/>
     </row>
-    <row r="236" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="236" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C236" s="1"/>
     </row>
-    <row r="237" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="237" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C237" s="1"/>
     </row>
-    <row r="238" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="238" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C238" s="1"/>
     </row>
-    <row r="239" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="239" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C239" s="1"/>
     </row>
-    <row r="240" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="240" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C240" s="1"/>
     </row>
-    <row r="241" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="241" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C241" s="1"/>
     </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="242" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C242" s="1"/>
     </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="243" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C243" s="1"/>
     </row>
-    <row r="244" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="244" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C244" s="1"/>
     </row>
-    <row r="245" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="245" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C245" s="1"/>
     </row>
-    <row r="246" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="246" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C246" s="1"/>
     </row>
-    <row r="247" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="247" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C247" s="1"/>
     </row>
-    <row r="248" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="248" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C248" s="1"/>
     </row>
-    <row r="249" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="249" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C249" s="1"/>
     </row>
-    <row r="250" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="250" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C250" s="1"/>
     </row>
-    <row r="251" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="251" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C251" s="1"/>
     </row>
-    <row r="252" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="252" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C252" s="1"/>
     </row>
-    <row r="253" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="253" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C253" s="1"/>
     </row>
-    <row r="254" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="254" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C254" s="1"/>
     </row>
-    <row r="255" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="255" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C255" s="1"/>
     </row>
-    <row r="256" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="256" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C256" s="1"/>
     </row>
-    <row r="257" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="257" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C257" s="1"/>
     </row>
-    <row r="258" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="258" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C258" s="1"/>
     </row>
-    <row r="259" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="259" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C259" s="1"/>
     </row>
-    <row r="260" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="260" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C260" s="1"/>
     </row>
-    <row r="261" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="261" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C261" s="1"/>
     </row>
-    <row r="262" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="262" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C262" s="1"/>
     </row>
-    <row r="263" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="263" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C263" s="1"/>
     </row>
-    <row r="264" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="264" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C264" s="1"/>
     </row>
-    <row r="265" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="265" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C265" s="1"/>
     </row>
-    <row r="266" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="266" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C266" s="1"/>
     </row>
-    <row r="267" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="267" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C267" s="1"/>
     </row>
-    <row r="268" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="268" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C268" s="1"/>
     </row>
-    <row r="269" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="269" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C269" s="1"/>
     </row>
-    <row r="270" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="270" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C270" s="1"/>
     </row>
-    <row r="271" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="271" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C271" s="1"/>
     </row>
-    <row r="272" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="272" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C272" s="1"/>
     </row>
-    <row r="273" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="273" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C273" s="1"/>
     </row>
-    <row r="274" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="274" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C274" s="1"/>
     </row>
-    <row r="275" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="275" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C275" s="1"/>
     </row>
-    <row r="276" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="276" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C276" s="1"/>
     </row>
-    <row r="277" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="277" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C277" s="1"/>
     </row>
-    <row r="278" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="278" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C278" s="1"/>
     </row>
-    <row r="279" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="279" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C279" s="1"/>
     </row>
-    <row r="280" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="280" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C280" s="1"/>
     </row>
-    <row r="281" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="281" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C281" s="1"/>
     </row>
-    <row r="282" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="282" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C282" s="1"/>
     </row>
-    <row r="283" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="283" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C283" s="1"/>
     </row>
-    <row r="284" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="284" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C284" s="1"/>
     </row>
-    <row r="285" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="285" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C285" s="1"/>
     </row>
-    <row r="286" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="286" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C286" s="1"/>
     </row>
-    <row r="287" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="287" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C287" s="1"/>
     </row>
-    <row r="288" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="288" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C288" s="1"/>
     </row>
-    <row r="289" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="289" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C289" s="1"/>
     </row>
-    <row r="290" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="290" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C290" s="1"/>
     </row>
-    <row r="291" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="291" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C291" s="1"/>
     </row>
-    <row r="292" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="292" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C292" s="1"/>
     </row>
-    <row r="293" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="293" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C293" s="1"/>
     </row>
-    <row r="294" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="294" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C294" s="1"/>
     </row>
-    <row r="295" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="295" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C295" s="1"/>
     </row>
-    <row r="296" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="296" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C296" s="1"/>
     </row>
-    <row r="297" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="297" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C297" s="1"/>
     </row>
-    <row r="298" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="298" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C298" s="1"/>
     </row>
-    <row r="299" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="299" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C299" s="1"/>
     </row>
-    <row r="300" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="300" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C300" s="1"/>
     </row>
-    <row r="301" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="301" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C301" s="1"/>
     </row>
-    <row r="302" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="302" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C302" s="1"/>
     </row>
-    <row r="303" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="303" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C303" s="1"/>
     </row>
-    <row r="304" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="304" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C304" s="1"/>
     </row>
-    <row r="305" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="305" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C305" s="1"/>
     </row>
-    <row r="306" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="306" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C306" s="1"/>
     </row>
-    <row r="307" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="307" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C307" s="1"/>
     </row>
-    <row r="308" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="308" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C308" s="1"/>
     </row>
-    <row r="309" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="309" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C309" s="1"/>
     </row>
-    <row r="310" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="310" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C310" s="1"/>
     </row>
-    <row r="311" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="311" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C311" s="1"/>
     </row>
-    <row r="312" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="312" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C312" s="2"/>
     </row>
-    <row r="313" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="313" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C313" s="2"/>
     </row>
-    <row r="314" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="314" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C314" s="2"/>
     </row>
-    <row r="315" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="315" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C315" s="2"/>
     </row>
-    <row r="316" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="316" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C316" s="2"/>
     </row>
-    <row r="317" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="317" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C317" s="2"/>
     </row>
-    <row r="318" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="318" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C318" s="2"/>
     </row>
-    <row r="319" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="319" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C319" s="2"/>
     </row>
-    <row r="320" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="320" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C320" s="2"/>
     </row>
-    <row r="321" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="321" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C321" s="2"/>
     </row>
-    <row r="322" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="322" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C322" s="2"/>
     </row>
-    <row r="323" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="323" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C323" s="2"/>
     </row>
-    <row r="324" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="324" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C324" s="2"/>
     </row>
-    <row r="325" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="325" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C325" s="2"/>
     </row>
-    <row r="326" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="326" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C326" s="2"/>
     </row>
-    <row r="327" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="327" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C327" s="2"/>
     </row>
-    <row r="328" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="328" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C328" s="2"/>
     </row>
-    <row r="329" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="329" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C329" s="2"/>
     </row>
-    <row r="330" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="330" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C330" s="2"/>
     </row>
-    <row r="331" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="331" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C331" s="2"/>
     </row>
-    <row r="332" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="332" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C332" s="2"/>
     </row>
-    <row r="333" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="333" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C333" s="2"/>
     </row>
-    <row r="334" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="334" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C334" s="2"/>
     </row>
-    <row r="335" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="335" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C335" s="2"/>
     </row>
-    <row r="336" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="336" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C336" s="2"/>
     </row>
   </sheetData>

</xml_diff>